<commit_message>
AD3-410 Add a way to handle Indicator Groups
</commit_message>
<xml_diff>
--- a/forms/src/main/resources/org/devgateway/toolkit/forms/wicket/page/edit/gisDepartmentDataset-Template.xlsx
+++ b/forms/src/main/resources/org/devgateway/toolkit/forms/wicket/page/edit/gisDepartmentDataset-Template.xlsx
@@ -22,12 +22,147 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t xml:space="preserve">Department Name</t>
   </si>
   <si>
     <t xml:space="preserve">Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bakel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bambey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bignona</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Birkilane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bounkiling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dagana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dakar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diourbel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fatick</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Foundiougne</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gossas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Goudiry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Goudomp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guinguinéo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guédiawaye</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kaffrine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kanel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kaolack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kolda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Koumpentoum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kounghel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kébémer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kédougou</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Linguère</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Louga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M'bour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Malem-Hodar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Matam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mbacké</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Médina Yoro Foulah</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nioro du Rip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oussouye</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pikine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Podor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ranérou</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rufisque</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saint-Louis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salemata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saraya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sédhiou</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tambacounda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thiès</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tivaouane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vélingara</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ziguinchor</t>
   </si>
 </sst>
 </file>
@@ -37,7 +172,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -61,19 +196,32 @@
       <family val="0"/>
     </font>
     <font>
+      <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCCCCC"/>
+        <bgColor rgb="FFCCCCFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -110,12 +258,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -128,6 +280,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFCCCCCC"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -136,10 +348,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -149,12 +361,237 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>